<commit_message>
Vote verification : Generate Excel file of Votes with verification
</commit_message>
<xml_diff>
--- a/passwords.xlsx
+++ b/passwords.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>a7e24fcd052d2b0f6f87</t>
-  </si>
-  <si>
-    <t>76104c8a99e4ddbd005b</t>
-  </si>
-  <si>
-    <t>0152fd6be132236a42f8</t>
-  </si>
-  <si>
-    <t>024dde171f641c988acd</t>
+    <t>fdec4c2032023fdccca6</t>
+  </si>
+  <si>
+    <t>b40965018b5ec67fbf48</t>
+  </si>
+  <si>
+    <t>0129c39d3efddff7cd09</t>
+  </si>
+  <si>
+    <t>db42be9ae6c37108dc0f</t>
   </si>
   <si>
     <t>kayush@iitg.ernet.in</t>

</xml_diff>